<commit_message>
Google drive name update
Updated template names for it too work
fixed readonly text box in info sheet tab
</commit_message>
<xml_diff>
--- a/Restored To Eden/InformationSheet.xlsx
+++ b/Restored To Eden/InformationSheet.xlsx
@@ -31,10 +31,10 @@
     <t>Our promises to you</t>
   </si>
   <si>
+    <t>Used By &amp; Best Before Date</t>
+  </si>
+  <si>
     <t>Ingredients</t>
-  </si>
-  <si>
-    <t>Used By &amp; Best Before Date</t>
   </si>
   <si>
     <t>AutoFilled by system</t>
@@ -456,10 +456,10 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>